<commit_message>
classes and elements added
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/CucumberTestResults.xlsx
+++ b/src/test/java/apachePOI/resource/CucumberTestResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>Login with valid username and password Passed</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t>Create a Country 2 Failed</t>
+  </si>
+  <si>
+    <t>Adding and removing items from the shopping cart Failed</t>
+  </si>
+  <si>
+    <t>Adding and removing items from the shopping cart Passed</t>
   </si>
 </sst>
 </file>
@@ -68,7 +74,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -124,6 +130,46 @@
         <v>3</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>